<commit_message>
edit personal.xlsx -add sample personal info
</commit_message>
<xml_diff>
--- a/xl/전체물품리스트_세트저장용.xlsx
+++ b/xl/전체물품리스트_세트저장용.xlsx
@@ -442,7 +442,7 @@
         <v>780</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -621,7 +621,7 @@
         <v>2000</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
@@ -674,7 +674,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -748,7 +748,7 @@
         <v>4000</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">

</xml_diff>